<commit_message>
project 2 is finished
</commit_message>
<xml_diff>
--- a/Project 2/winding.xlsx
+++ b/Project 2/winding.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="33">
   <si>
     <t>A1</t>
   </si>
@@ -96,6 +96,33 @@
   </si>
   <si>
     <t>B4</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Third</t>
+  </si>
+  <si>
+    <t>Fifth</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>-B</t>
+  </si>
+  <si>
+    <t>-C</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>-A</t>
   </si>
 </sst>
 </file>
@@ -112,15 +139,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -249,15 +294,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -289,6 +368,48 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -571,133 +692,1883 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="B1:AZ29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R32" sqref="R32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="12" width="7.140625" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="7.140625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.28515625" style="12" customWidth="1"/>
+    <col min="4" max="14" width="4" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="26" width="4" style="12" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="3" style="12" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="4" style="12" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="3" style="12" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="4" style="12" bestFit="1" customWidth="1"/>
+    <col min="33" max="36" width="9.140625" style="12"/>
+    <col min="37" max="37" width="5.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="3.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="39" max="49" width="4.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="3.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="51" max="52" width="4.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="53" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="2">
+    <row r="1" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="B1" s="1">
         <v>1</v>
       </c>
-      <c r="B1" s="3">
+      <c r="C1" s="2">
         <v>2</v>
       </c>
-      <c r="C1" s="3">
+      <c r="D1" s="2">
         <v>3</v>
       </c>
-      <c r="D1" s="3">
+      <c r="E1" s="2">
         <v>4</v>
       </c>
-      <c r="E1" s="3">
+      <c r="F1" s="2">
         <v>5</v>
       </c>
-      <c r="F1" s="3">
+      <c r="G1" s="2">
         <v>6</v>
       </c>
-      <c r="G1" s="3">
+      <c r="H1" s="2">
         <v>7</v>
       </c>
-      <c r="H1" s="3">
+      <c r="I1" s="2">
         <v>8</v>
       </c>
-      <c r="I1" s="3">
+      <c r="J1" s="2">
         <v>9</v>
       </c>
-      <c r="J1" s="3">
+      <c r="K1" s="2">
         <v>10</v>
       </c>
-      <c r="K1" s="3">
+      <c r="L1" s="2">
         <v>11</v>
       </c>
-      <c r="L1" s="4">
+      <c r="M1" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="L2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="M2" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="2:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="H3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="I3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="J3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="K3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="L3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="M3" s="11" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="B5" s="15"/>
+      <c r="C5" s="16">
+        <v>1</v>
+      </c>
+      <c r="D5" s="16">
+        <v>2</v>
+      </c>
+      <c r="E5" s="16">
+        <v>3</v>
+      </c>
+      <c r="F5" s="16">
+        <v>4</v>
+      </c>
+      <c r="G5" s="16">
+        <v>5</v>
+      </c>
+      <c r="H5" s="16">
+        <v>6</v>
+      </c>
+      <c r="I5" s="16">
+        <v>7</v>
+      </c>
+      <c r="J5" s="16">
+        <v>8</v>
+      </c>
+      <c r="K5" s="16">
+        <v>9</v>
+      </c>
+      <c r="L5" s="16">
+        <v>10</v>
+      </c>
+      <c r="M5" s="16">
+        <v>11</v>
+      </c>
+      <c r="N5" s="16">
+        <v>12</v>
+      </c>
+      <c r="O5" s="16">
+        <v>13</v>
+      </c>
+      <c r="P5" s="16">
+        <v>14</v>
+      </c>
+      <c r="Q5" s="16">
+        <v>15</v>
+      </c>
+      <c r="R5" s="16">
+        <v>16</v>
+      </c>
+      <c r="S5" s="16">
+        <v>17</v>
+      </c>
+      <c r="T5" s="16">
+        <v>18</v>
+      </c>
+      <c r="U5" s="16">
+        <v>19</v>
+      </c>
+      <c r="V5" s="16">
+        <v>20</v>
+      </c>
+      <c r="W5" s="16">
+        <v>21</v>
+      </c>
+      <c r="X5" s="16">
+        <v>22</v>
+      </c>
+      <c r="Y5" s="16">
+        <v>23</v>
+      </c>
+      <c r="Z5" s="16">
+        <v>24</v>
+      </c>
+      <c r="AA5" s="16">
+        <v>25</v>
+      </c>
+      <c r="AB5" s="16">
+        <v>26</v>
+      </c>
+      <c r="AC5" s="16">
+        <v>27</v>
+      </c>
+      <c r="AD5" s="16">
+        <v>28</v>
+      </c>
+      <c r="AE5" s="16">
+        <v>29</v>
+      </c>
+      <c r="AF5" s="17">
+        <v>30</v>
+      </c>
+      <c r="AK5" s="15"/>
+      <c r="AL5" s="16">
+        <v>1</v>
+      </c>
+      <c r="AM5" s="16">
+        <v>2</v>
+      </c>
+      <c r="AN5" s="16">
+        <v>3</v>
+      </c>
+      <c r="AO5" s="16">
+        <v>4</v>
+      </c>
+      <c r="AP5" s="16">
+        <v>5</v>
+      </c>
+      <c r="AQ5" s="16">
+        <v>6</v>
+      </c>
+      <c r="AR5" s="16">
+        <v>7</v>
+      </c>
+      <c r="AS5" s="16">
+        <v>8</v>
+      </c>
+      <c r="AT5" s="16">
+        <v>9</v>
+      </c>
+      <c r="AU5" s="16">
+        <v>10</v>
+      </c>
+      <c r="AV5" s="16">
+        <v>11</v>
+      </c>
+      <c r="AW5" s="16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>120</v>
+      </c>
+      <c r="E6" s="5">
+        <v>240</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
+        <v>120</v>
+      </c>
+      <c r="H6" s="5">
+        <v>240</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
+      <c r="J6" s="5">
+        <v>120</v>
+      </c>
+      <c r="K6" s="5">
+        <v>240</v>
+      </c>
+      <c r="L6" s="5">
+        <v>0</v>
+      </c>
+      <c r="M6" s="5">
+        <v>120</v>
+      </c>
+      <c r="N6" s="5">
+        <v>240</v>
+      </c>
+      <c r="O6" s="5">
+        <v>0</v>
+      </c>
+      <c r="P6" s="5">
+        <v>120</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>240</v>
+      </c>
+      <c r="R6" s="5">
+        <v>0</v>
+      </c>
+      <c r="S6" s="5">
+        <v>120</v>
+      </c>
+      <c r="T6" s="5">
+        <v>240</v>
+      </c>
+      <c r="U6" s="5">
+        <v>0</v>
+      </c>
+      <c r="V6" s="5">
+        <v>120</v>
+      </c>
+      <c r="W6" s="5">
+        <v>240</v>
+      </c>
+      <c r="X6" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="5">
+        <v>120</v>
+      </c>
+      <c r="Z6" s="5">
+        <v>240</v>
+      </c>
+      <c r="AA6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="5">
+        <v>120</v>
+      </c>
+      <c r="AC6" s="5">
+        <v>240</v>
+      </c>
+      <c r="AD6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="5">
+        <v>120</v>
+      </c>
+      <c r="AF6" s="13">
+        <v>240</v>
+      </c>
+      <c r="AK6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AL6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="5">
+        <v>150</v>
+      </c>
+      <c r="AN6" s="5">
+        <v>300</v>
+      </c>
+      <c r="AO6" s="5">
+        <v>90</v>
+      </c>
+      <c r="AP6" s="5">
+        <v>240</v>
+      </c>
+      <c r="AQ6" s="5">
+        <v>30</v>
+      </c>
+      <c r="AR6" s="5">
+        <v>180</v>
+      </c>
+      <c r="AS6" s="5">
+        <v>330</v>
+      </c>
+      <c r="AT6" s="5">
+        <v>120</v>
+      </c>
+      <c r="AU6" s="5">
+        <v>270</v>
+      </c>
+      <c r="AV6" s="5">
+        <v>60</v>
+      </c>
+      <c r="AW6" s="5">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="7" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0</v>
+      </c>
+      <c r="J7" s="5">
+        <v>0</v>
+      </c>
+      <c r="K7" s="5">
+        <v>0</v>
+      </c>
+      <c r="L7" s="5">
+        <v>0</v>
+      </c>
+      <c r="M7" s="5">
+        <v>0</v>
+      </c>
+      <c r="N7" s="5">
+        <v>0</v>
+      </c>
+      <c r="O7" s="5">
+        <v>0</v>
+      </c>
+      <c r="P7" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>0</v>
+      </c>
+      <c r="R7" s="5">
+        <v>0</v>
+      </c>
+      <c r="S7" s="5">
+        <v>0</v>
+      </c>
+      <c r="T7" s="5">
+        <v>0</v>
+      </c>
+      <c r="U7" s="5">
+        <v>0</v>
+      </c>
+      <c r="V7" s="5">
+        <v>0</v>
+      </c>
+      <c r="W7" s="5">
+        <v>0</v>
+      </c>
+      <c r="X7" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="13">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AL7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="5">
+        <v>90</v>
+      </c>
+      <c r="AN7" s="5">
+        <v>180</v>
+      </c>
+      <c r="AO7" s="5">
+        <v>270</v>
+      </c>
+      <c r="AP7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ7" s="5">
+        <v>90</v>
+      </c>
+      <c r="AR7" s="5">
+        <v>180</v>
+      </c>
+      <c r="AS7" s="5">
+        <v>270</v>
+      </c>
+      <c r="AT7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU7" s="5">
+        <v>90</v>
+      </c>
+      <c r="AV7" s="5">
+        <v>180</v>
+      </c>
+      <c r="AW7" s="5">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="8" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>240</v>
+      </c>
+      <c r="E8" s="5">
+        <v>120</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
+        <v>240</v>
+      </c>
+      <c r="H8" s="5">
+        <v>120</v>
+      </c>
+      <c r="I8" s="5">
+        <v>0</v>
+      </c>
+      <c r="J8" s="5">
+        <v>240</v>
+      </c>
+      <c r="K8" s="5">
+        <v>120</v>
+      </c>
+      <c r="L8" s="5">
+        <v>0</v>
+      </c>
+      <c r="M8" s="5">
+        <v>240</v>
+      </c>
+      <c r="N8" s="5">
+        <v>120</v>
+      </c>
+      <c r="O8" s="5">
+        <v>0</v>
+      </c>
+      <c r="P8" s="5">
+        <v>240</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>120</v>
+      </c>
+      <c r="R8" s="5">
+        <v>0</v>
+      </c>
+      <c r="S8" s="5">
+        <v>240</v>
+      </c>
+      <c r="T8" s="5">
+        <v>120</v>
+      </c>
+      <c r="U8" s="5">
+        <v>0</v>
+      </c>
+      <c r="V8" s="5">
+        <v>240</v>
+      </c>
+      <c r="W8" s="5">
+        <v>120</v>
+      </c>
+      <c r="X8" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="5">
+        <v>240</v>
+      </c>
+      <c r="Z8" s="5">
+        <v>120</v>
+      </c>
+      <c r="AA8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="5">
+        <v>240</v>
+      </c>
+      <c r="AC8" s="5">
+        <v>120</v>
+      </c>
+      <c r="AD8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="5">
+        <v>240</v>
+      </c>
+      <c r="AF8" s="13">
+        <v>120</v>
+      </c>
+      <c r="AK8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AL8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM8" s="5">
+        <v>30</v>
+      </c>
+      <c r="AN8" s="5">
+        <v>60</v>
+      </c>
+      <c r="AO8" s="5">
+        <v>90</v>
+      </c>
+      <c r="AP8" s="5">
+        <v>120</v>
+      </c>
+      <c r="AQ8" s="5">
+        <v>150</v>
+      </c>
+      <c r="AR8" s="5">
+        <v>180</v>
+      </c>
+      <c r="AS8" s="5">
+        <v>210</v>
+      </c>
+      <c r="AT8" s="5">
+        <v>240</v>
+      </c>
+      <c r="AU8" s="5">
+        <v>270</v>
+      </c>
+      <c r="AV8" s="5">
+        <v>300</v>
+      </c>
+      <c r="AW8" s="5">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="9" spans="2:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="8"/>
+      <c r="C9" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="M9" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="O9" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="P9" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q9" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="R9" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="S9" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="T9" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="U9" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="V9" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="W9" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="X9" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y9" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z9" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA9" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB9" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC9" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD9" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE9" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF9" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="AK9" s="8"/>
+      <c r="AL9" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="AM9" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN9" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO9" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="AP9" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="AQ9" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="AR9" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="AS9" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="AT9" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="AU9" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="AV9" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="AW9" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="2:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="2:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AL11" s="16">
+        <v>13</v>
+      </c>
+      <c r="AM11" s="16">
+        <v>14</v>
+      </c>
+      <c r="AN11" s="16">
+        <v>15</v>
+      </c>
+      <c r="AO11" s="16">
+        <v>16</v>
+      </c>
+      <c r="AP11" s="16">
+        <v>17</v>
+      </c>
+      <c r="AQ11" s="16">
+        <v>18</v>
+      </c>
+      <c r="AR11" s="16">
+        <v>19</v>
+      </c>
+      <c r="AS11" s="16">
+        <v>20</v>
+      </c>
+      <c r="AT11" s="16">
+        <v>21</v>
+      </c>
+      <c r="AU11" s="16">
+        <v>22</v>
+      </c>
+      <c r="AV11" s="16">
+        <v>23</v>
+      </c>
+      <c r="AW11" s="17">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="B12" s="15"/>
+      <c r="C12" s="16">
+        <v>1</v>
+      </c>
+      <c r="D12" s="16">
+        <v>2</v>
+      </c>
+      <c r="E12" s="16">
+        <v>3</v>
+      </c>
+      <c r="F12" s="16">
+        <v>4</v>
+      </c>
+      <c r="G12" s="16">
+        <v>5</v>
+      </c>
+      <c r="H12" s="16">
+        <v>6</v>
+      </c>
+      <c r="I12" s="16">
+        <v>7</v>
+      </c>
+      <c r="J12" s="16">
+        <v>8</v>
+      </c>
+      <c r="K12" s="16">
+        <v>9</v>
+      </c>
+      <c r="L12" s="16">
+        <v>10</v>
+      </c>
+      <c r="M12" s="16">
+        <v>11</v>
+      </c>
+      <c r="N12" s="16">
+        <v>12</v>
+      </c>
+      <c r="O12" s="16">
+        <v>13</v>
+      </c>
+      <c r="P12" s="16">
+        <v>14</v>
+      </c>
+      <c r="Q12" s="16">
+        <v>15</v>
+      </c>
+      <c r="R12" s="16">
+        <v>16</v>
+      </c>
+      <c r="S12" s="16">
+        <v>17</v>
+      </c>
+      <c r="T12" s="16">
+        <v>18</v>
+      </c>
+      <c r="U12" s="16">
+        <v>19</v>
+      </c>
+      <c r="V12" s="16">
+        <v>20</v>
+      </c>
+      <c r="W12" s="16">
+        <v>21</v>
+      </c>
+      <c r="X12" s="16">
+        <v>22</v>
+      </c>
+      <c r="Y12" s="16">
+        <v>23</v>
+      </c>
+      <c r="Z12" s="17">
+        <v>24</v>
+      </c>
+      <c r="AA12" s="14"/>
+      <c r="AB12" s="14"/>
+      <c r="AC12" s="14"/>
+      <c r="AD12" s="14"/>
+      <c r="AE12" s="14"/>
+      <c r="AF12" s="14"/>
+      <c r="AL12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM12" s="5">
+        <v>150</v>
+      </c>
+      <c r="AN12" s="5">
+        <v>300</v>
+      </c>
+      <c r="AO12" s="5">
+        <v>90</v>
+      </c>
+      <c r="AP12" s="5">
+        <v>240</v>
+      </c>
+      <c r="AQ12" s="5">
+        <v>30</v>
+      </c>
+      <c r="AR12" s="5">
+        <v>180</v>
+      </c>
+      <c r="AS12" s="5">
+        <v>330</v>
+      </c>
+      <c r="AT12" s="5">
+        <v>120</v>
+      </c>
+      <c r="AU12" s="5">
+        <v>270</v>
+      </c>
+      <c r="AV12" s="5">
+        <v>60</v>
+      </c>
+      <c r="AW12" s="13">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="13" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5">
+        <v>150</v>
+      </c>
+      <c r="E13" s="5">
+        <v>300</v>
+      </c>
+      <c r="F13" s="5">
+        <v>90</v>
+      </c>
+      <c r="G13" s="5">
+        <v>240</v>
+      </c>
+      <c r="H13" s="5">
+        <v>30</v>
+      </c>
+      <c r="I13" s="5">
+        <v>180</v>
+      </c>
+      <c r="J13" s="5">
+        <v>330</v>
+      </c>
+      <c r="K13" s="5">
+        <v>120</v>
+      </c>
+      <c r="L13" s="5">
+        <v>270</v>
+      </c>
+      <c r="M13" s="5">
+        <v>60</v>
+      </c>
+      <c r="N13" s="5">
+        <v>210</v>
+      </c>
+      <c r="O13" s="5">
+        <v>0</v>
+      </c>
+      <c r="P13" s="5">
+        <v>150</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>300</v>
+      </c>
+      <c r="R13" s="5">
+        <v>90</v>
+      </c>
+      <c r="S13" s="5">
+        <v>240</v>
+      </c>
+      <c r="T13" s="5">
+        <v>30</v>
+      </c>
+      <c r="U13" s="5">
+        <v>180</v>
+      </c>
+      <c r="V13" s="5">
+        <v>330</v>
+      </c>
+      <c r="W13" s="5">
+        <v>120</v>
+      </c>
+      <c r="X13" s="5">
+        <v>270</v>
+      </c>
+      <c r="Y13" s="5">
+        <v>60</v>
+      </c>
+      <c r="Z13" s="13">
+        <v>210</v>
+      </c>
+      <c r="AA13" s="14"/>
+      <c r="AB13" s="14"/>
+      <c r="AC13" s="14"/>
+      <c r="AD13" s="14"/>
+      <c r="AE13" s="14"/>
+      <c r="AF13" s="14"/>
+      <c r="AL13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM13" s="5">
+        <v>90</v>
+      </c>
+      <c r="AN13" s="5">
+        <v>180</v>
+      </c>
+      <c r="AO13" s="5">
+        <v>270</v>
+      </c>
+      <c r="AP13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ13" s="5">
+        <v>90</v>
+      </c>
+      <c r="AR13" s="5">
+        <v>180</v>
+      </c>
+      <c r="AS13" s="5">
+        <v>270</v>
+      </c>
+      <c r="AT13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU13" s="5">
+        <v>90</v>
+      </c>
+      <c r="AV13" s="5">
+        <v>180</v>
+      </c>
+      <c r="AW13" s="13">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="14" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0</v>
+      </c>
+      <c r="D14" s="5">
+        <v>90</v>
+      </c>
+      <c r="E14" s="5">
+        <v>180</v>
+      </c>
+      <c r="F14" s="5">
+        <v>270</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0</v>
+      </c>
+      <c r="H14" s="5">
+        <v>90</v>
+      </c>
+      <c r="I14" s="5">
+        <v>180</v>
+      </c>
+      <c r="J14" s="5">
+        <v>270</v>
+      </c>
+      <c r="K14" s="5">
+        <v>0</v>
+      </c>
+      <c r="L14" s="5">
+        <v>90</v>
+      </c>
+      <c r="M14" s="5">
+        <v>180</v>
+      </c>
+      <c r="N14" s="5">
+        <v>270</v>
+      </c>
+      <c r="O14" s="5">
+        <v>0</v>
+      </c>
+      <c r="P14" s="5">
+        <v>90</v>
+      </c>
+      <c r="Q14" s="5">
+        <v>180</v>
+      </c>
+      <c r="R14" s="5">
+        <v>270</v>
+      </c>
+      <c r="S14" s="5">
+        <v>0</v>
+      </c>
+      <c r="T14" s="5">
+        <v>90</v>
+      </c>
+      <c r="U14" s="5">
+        <v>180</v>
+      </c>
+      <c r="V14" s="5">
+        <v>270</v>
+      </c>
+      <c r="W14" s="5">
+        <v>0</v>
+      </c>
+      <c r="X14" s="5">
+        <v>90</v>
+      </c>
+      <c r="Y14" s="5">
+        <v>180</v>
+      </c>
+      <c r="Z14" s="13">
+        <v>270</v>
+      </c>
+      <c r="AA14" s="14"/>
+      <c r="AB14" s="14"/>
+      <c r="AC14" s="14"/>
+      <c r="AD14" s="14"/>
+      <c r="AE14" s="14"/>
+      <c r="AF14" s="14"/>
+      <c r="AL14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM14" s="5">
+        <v>30</v>
+      </c>
+      <c r="AN14" s="5">
+        <v>60</v>
+      </c>
+      <c r="AO14" s="5">
+        <v>90</v>
+      </c>
+      <c r="AP14" s="5">
+        <v>120</v>
+      </c>
+      <c r="AQ14" s="5">
+        <v>150</v>
+      </c>
+      <c r="AR14" s="5">
+        <v>180</v>
+      </c>
+      <c r="AS14" s="5">
+        <v>210</v>
+      </c>
+      <c r="AT14" s="5">
+        <v>240</v>
+      </c>
+      <c r="AU14" s="5">
+        <v>270</v>
+      </c>
+      <c r="AV14" s="5">
+        <v>300</v>
+      </c>
+      <c r="AW14" s="13">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="15" spans="2:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0</v>
+      </c>
+      <c r="D15" s="5">
+        <v>30</v>
+      </c>
+      <c r="E15" s="5">
+        <v>60</v>
+      </c>
+      <c r="F15" s="5">
+        <v>90</v>
+      </c>
+      <c r="G15" s="5">
+        <v>120</v>
+      </c>
+      <c r="H15" s="5">
+        <v>150</v>
+      </c>
+      <c r="I15" s="5">
+        <v>180</v>
+      </c>
+      <c r="J15" s="5">
+        <v>210</v>
+      </c>
+      <c r="K15" s="5">
+        <v>240</v>
+      </c>
+      <c r="L15" s="5">
+        <v>270</v>
+      </c>
+      <c r="M15" s="5">
+        <v>300</v>
+      </c>
+      <c r="N15" s="5">
+        <v>330</v>
+      </c>
+      <c r="O15" s="5">
+        <v>0</v>
+      </c>
+      <c r="P15" s="5">
+        <v>30</v>
+      </c>
+      <c r="Q15" s="5">
+        <v>60</v>
+      </c>
+      <c r="R15" s="5">
+        <v>90</v>
+      </c>
+      <c r="S15" s="5">
+        <v>120</v>
+      </c>
+      <c r="T15" s="5">
+        <v>150</v>
+      </c>
+      <c r="U15" s="5">
+        <v>180</v>
+      </c>
+      <c r="V15" s="5">
+        <v>210</v>
+      </c>
+      <c r="W15" s="5">
+        <v>240</v>
+      </c>
+      <c r="X15" s="5">
+        <v>270</v>
+      </c>
+      <c r="Y15" s="5">
+        <v>300</v>
+      </c>
+      <c r="Z15" s="13">
+        <v>330</v>
+      </c>
+      <c r="AA15" s="14"/>
+      <c r="AB15" s="14"/>
+      <c r="AC15" s="14"/>
+      <c r="AD15" s="14"/>
+      <c r="AE15" s="14"/>
+      <c r="AF15" s="14"/>
+      <c r="AL15" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="AM15" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN15" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO15" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="AP15" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="AQ15" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="AR15" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="AS15" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="AT15" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="AU15" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="AV15" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="AW15" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="2:49" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="8"/>
+      <c r="C16" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="J16" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K16" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="L16" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="M16" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="N16" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="O16" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="P16" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q16" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="R16" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="S16" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="T16" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="U16" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="V16" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="W16" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="X16" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y16" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z16" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="37:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="37:52" x14ac:dyDescent="0.25">
+      <c r="AK19" s="15"/>
+      <c r="AL19" s="16">
+        <v>1</v>
+      </c>
+      <c r="AM19" s="16">
+        <v>2</v>
+      </c>
+      <c r="AN19" s="16">
+        <v>3</v>
+      </c>
+      <c r="AO19" s="16">
+        <v>4</v>
+      </c>
+      <c r="AP19" s="16">
+        <v>5</v>
+      </c>
+      <c r="AQ19" s="16">
+        <v>6</v>
+      </c>
+      <c r="AR19" s="16">
+        <v>7</v>
+      </c>
+      <c r="AS19" s="16">
+        <v>8</v>
+      </c>
+      <c r="AT19" s="16">
+        <v>9</v>
+      </c>
+      <c r="AU19" s="16">
+        <v>10</v>
+      </c>
+      <c r="AV19" s="16">
+        <v>11</v>
+      </c>
+      <c r="AW19" s="16">
+        <v>12</v>
+      </c>
+      <c r="AX19" s="16">
+        <v>13</v>
+      </c>
+      <c r="AY19" s="16">
+        <v>14</v>
+      </c>
+      <c r="AZ19" s="16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="37:52" x14ac:dyDescent="0.25">
+      <c r="AK20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AL20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM20" s="5">
+        <v>120</v>
+      </c>
+      <c r="AN20" s="5">
+        <v>240</v>
+      </c>
+      <c r="AO20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP20" s="5">
+        <v>120</v>
+      </c>
+      <c r="AQ20" s="5">
+        <v>240</v>
+      </c>
+      <c r="AR20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS20" s="5">
+        <v>120</v>
+      </c>
+      <c r="AT20" s="5">
+        <v>240</v>
+      </c>
+      <c r="AU20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV20" s="5">
+        <v>120</v>
+      </c>
+      <c r="AW20" s="5">
+        <v>240</v>
+      </c>
+      <c r="AX20" s="5">
+        <v>0</v>
+      </c>
+      <c r="AY20" s="5">
+        <v>120</v>
+      </c>
+      <c r="AZ20" s="5">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="21" spans="37:52" x14ac:dyDescent="0.25">
+      <c r="AK21" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AL21" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM21" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN21" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO21" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP21" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ21" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR21" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS21" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT21" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU21" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV21" s="5">
+        <v>0</v>
+      </c>
+      <c r="AW21" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX21" s="5">
+        <v>0</v>
+      </c>
+      <c r="AY21" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ21" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="37:52" x14ac:dyDescent="0.25">
+      <c r="AK22" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AL22" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM22" s="5">
+        <v>240</v>
+      </c>
+      <c r="AN22" s="5">
+        <v>120</v>
+      </c>
+      <c r="AO22" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP22" s="5">
+        <v>240</v>
+      </c>
+      <c r="AQ22" s="5">
+        <v>120</v>
+      </c>
+      <c r="AR22" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS22" s="5">
+        <v>240</v>
+      </c>
+      <c r="AT22" s="5">
+        <v>120</v>
+      </c>
+      <c r="AU22" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV22" s="5">
+        <v>240</v>
+      </c>
+      <c r="AW22" s="5">
+        <v>120</v>
+      </c>
+      <c r="AX22" s="5">
+        <v>0</v>
+      </c>
+      <c r="AY22" s="5">
+        <v>240</v>
+      </c>
+      <c r="AZ22" s="5">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="37:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AK23" s="8"/>
+      <c r="AL23" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="AM23" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN23" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="AO23" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP23" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="AQ23" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="AR23" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="AS23" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="AT23" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="AU23" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="AV23" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW23" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="AX23" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="AY23" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="AZ23" s="24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="37:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="37:52" x14ac:dyDescent="0.25">
+      <c r="AL25" s="16">
+        <v>16</v>
+      </c>
+      <c r="AM25" s="16">
+        <v>17</v>
+      </c>
+      <c r="AN25" s="16">
+        <v>18</v>
+      </c>
+      <c r="AO25" s="16">
+        <v>19</v>
+      </c>
+      <c r="AP25" s="16">
+        <v>20</v>
+      </c>
+      <c r="AQ25" s="16">
+        <v>21</v>
+      </c>
+      <c r="AR25" s="16">
+        <v>22</v>
+      </c>
+      <c r="AS25" s="16">
+        <v>23</v>
+      </c>
+      <c r="AT25" s="16">
+        <v>24</v>
+      </c>
+      <c r="AU25" s="16">
+        <v>25</v>
+      </c>
+      <c r="AV25" s="16">
+        <v>26</v>
+      </c>
+      <c r="AW25" s="16">
+        <v>27</v>
+      </c>
+      <c r="AX25" s="16">
+        <v>28</v>
+      </c>
+      <c r="AY25" s="16">
+        <v>29</v>
+      </c>
+      <c r="AZ25" s="17">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="37:52" x14ac:dyDescent="0.25">
+      <c r="AL26" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM26" s="5">
+        <v>120</v>
+      </c>
+      <c r="AN26" s="5">
+        <v>240</v>
+      </c>
+      <c r="AO26" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP26" s="5">
+        <v>120</v>
+      </c>
+      <c r="AQ26" s="5">
+        <v>240</v>
+      </c>
+      <c r="AR26" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS26" s="5">
+        <v>120</v>
+      </c>
+      <c r="AT26" s="5">
+        <v>240</v>
+      </c>
+      <c r="AU26" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV26" s="5">
+        <v>120</v>
+      </c>
+      <c r="AW26" s="5">
+        <v>240</v>
+      </c>
+      <c r="AX26" s="5">
+        <v>0</v>
+      </c>
+      <c r="AY26" s="5">
+        <v>120</v>
+      </c>
+      <c r="AZ26" s="13">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="27" spans="37:52" x14ac:dyDescent="0.25">
+      <c r="AL27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AW27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AY27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ27" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="37:52" x14ac:dyDescent="0.25">
+      <c r="AL28" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM28" s="5">
+        <v>240</v>
+      </c>
+      <c r="AN28" s="5">
+        <v>120</v>
+      </c>
+      <c r="AO28" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP28" s="5">
+        <v>240</v>
+      </c>
+      <c r="AQ28" s="5">
+        <v>120</v>
+      </c>
+      <c r="AR28" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS28" s="5">
+        <v>240</v>
+      </c>
+      <c r="AT28" s="5">
+        <v>120</v>
+      </c>
+      <c r="AU28" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV28" s="5">
+        <v>240</v>
+      </c>
+      <c r="AW28" s="5">
+        <v>120</v>
+      </c>
+      <c r="AX28" s="5">
+        <v>0</v>
+      </c>
+      <c r="AY28" s="5">
+        <v>240</v>
+      </c>
+      <c r="AZ28" s="13">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="37:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AL29" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="AM29" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN29" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="AO29" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="AP29" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="AQ29" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="AR29" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="AS29" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="AT29" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="AU29" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="AV29" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW29" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="AX29" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="AY29" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="AZ29" s="25" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>